<commit_message>
Added new TCs for 'MakeACopy'. along with it's function
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/makeACopy_newUI/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/makeACopy_newUI/TestData.xlsx
@@ -12,12 +12,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="70">
+  <si>
+    <t>Variable</t>
+  </si>
   <si>
     <t>Supported Browser Types</t>
   </si>
   <si>
-    <t>Variable</t>
+    <t>Data1</t>
+  </si>
+  <si>
+    <t>Data2</t>
+  </si>
+  <si>
+    <t>Data3</t>
+  </si>
+  <si>
+    <t>Data4</t>
+  </si>
+  <si>
+    <t>URL_login_login</t>
   </si>
   <si>
     <t>MozillaFirefox</t>
@@ -32,21 +47,6 @@
     <t>MicrosoftEdge</t>
   </si>
   <si>
-    <t>Data1</t>
-  </si>
-  <si>
-    <t>Data2</t>
-  </si>
-  <si>
-    <t>Data3</t>
-  </si>
-  <si>
-    <t>Data4</t>
-  </si>
-  <si>
-    <t>URL_login_login</t>
-  </si>
-  <si>
     <t>#/login</t>
   </si>
   <si>
@@ -113,18 +113,30 @@
     <t>Username</t>
   </si>
   <si>
-    <t>admin</t>
+    <t>Automation_Analyzer</t>
   </si>
   <si>
     <t>Password</t>
   </si>
   <si>
+    <t>Automation_Analyzer1</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
     <t>Automation_Dashboard_MakeACopyOptionDisplayed</t>
   </si>
   <si>
+    <t>New Dashboard</t>
+  </si>
+  <si>
     <t>Automation_Folder_ToCopyDashboardToIt</t>
   </si>
   <si>
+    <t>New Folder</t>
+  </si>
+  <si>
     <t>Automation_Dashboard_CopyAndOpen</t>
   </si>
   <si>
@@ -132,13 +144,91 @@
   </si>
   <si>
     <t>Automation_Dashboard_CancelCopy</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CopyDashboard_LongDashboardName</t>
+  </si>
+  <si>
+    <t>LongDashboardName</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CopyDashboard_LongDashboardNameAutomation_Dashboard_CopyDashboard_LongDashboardNameAutomation_Dashboard_CopyDashboard_LongDashboardNameAutomation_Dashboard_CopyDashboard_LongDashboardName</t>
+  </si>
+  <si>
+    <t>New Long Dashboard Name</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CopyDashboard_SpecialCharactersDashboardName</t>
+  </si>
+  <si>
+    <t>SpecialCharactersDashboardName</t>
+  </si>
+  <si>
+    <t>NewAutomation!@#$%^&amp;*()_+}{[]\';'/.,DashboardName</t>
+  </si>
+  <si>
+    <t>New special characters dashboard name</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CopyDashboard_ArabicName</t>
+  </si>
+  <si>
+    <t>ArabicDashboardName</t>
+  </si>
+  <si>
+    <t>لوحة التحكم الآلي</t>
+  </si>
+  <si>
+    <t>New Arabic Dashboard Name</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CopyDashboard_FrenchName</t>
+  </si>
+  <si>
+    <t>FrenchDashboardName</t>
+  </si>
+  <si>
+    <t>ĉĈćĆąăëêéèçàá</t>
+  </si>
+  <si>
+    <t>New French Dashboard Name</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CopyDashboard_ChineseName</t>
+  </si>
+  <si>
+    <t>ChineseDashboardName</t>
+  </si>
+  <si>
+    <t>汉字汉字漢字</t>
+  </si>
+  <si>
+    <t>New Chinese Dashboard Name</t>
+  </si>
+  <si>
+    <t>Automation_Folder_SharedEdit_ToAnalyzer</t>
+  </si>
+  <si>
+    <t>New Folder Created by admin and shared 'Edit' to analyzer</t>
+  </si>
+  <si>
+    <t>Automation_Folder_SharedView_ToAnalyzer</t>
+  </si>
+  <si>
+    <t>New Folder Created by admin and shared 'View' to analyzer</t>
+  </si>
+  <si>
+    <t>Automation_Folder_SharedShare_ToAnalyzer</t>
+  </si>
+  <si>
+    <t>New Folder Created by admin and shared 'Share' to analyzer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -161,8 +251,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,6 +273,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFC5E0B4"/>
         <bgColor rgb="FFC5E0B4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -238,15 +338,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -271,8 +371,35 @@
     <xf borderId="2" fillId="3" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="3" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -300,7 +427,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="53.14"/>
+    <col customWidth="1" min="1" max="1" width="58.43"/>
     <col customWidth="1" min="2" max="2" width="64.29"/>
     <col customWidth="1" min="3" max="3" width="36.14"/>
     <col customWidth="1" min="4" max="15" width="8.57"/>
@@ -308,35 +435,35 @@
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
     </row>
     <row r="2" ht="13.5" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>11</v>
@@ -610,7 +737,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -628,8 +755,10 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="A16" s="8"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="13" t="s">
+        <v>36</v>
+      </c>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
@@ -645,12 +774,14 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -666,12 +797,14 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -687,12 +820,14 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -708,12 +843,14 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="A20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="3"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -729,12 +866,14 @@
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="4"/>
+        <v>43</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -749,26 +888,38 @@
       <c r="O21" s="6"/>
     </row>
     <row r="22" ht="13.5" customHeight="1">
-      <c r="A22" s="12"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
+      <c r="A22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
     </row>
     <row r="23" ht="13.5" customHeight="1">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
+      <c r="A23" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -783,257 +934,855 @@
       <c r="O23" s="7"/>
     </row>
     <row r="24" ht="13.5" customHeight="1">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
+      <c r="A24" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="19"/>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="19"/>
+      <c r="T24" s="19"/>
+      <c r="U24" s="19"/>
+      <c r="V24" s="19"/>
+      <c r="W24" s="19"/>
+      <c r="X24" s="19"/>
+      <c r="Y24" s="19"/>
+      <c r="Z24" s="19"/>
     </row>
     <row r="25" ht="13.5" customHeight="1">
-      <c r="A25" s="12"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="7"/>
+      <c r="A25" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="19"/>
+      <c r="S25" s="19"/>
+      <c r="T25" s="19"/>
+      <c r="U25" s="19"/>
+      <c r="V25" s="19"/>
+      <c r="W25" s="19"/>
+      <c r="X25" s="19"/>
+      <c r="Y25" s="19"/>
+      <c r="Z25" s="19"/>
     </row>
     <row r="26" ht="13.5" customHeight="1">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="7"/>
-      <c r="O26" s="7"/>
+      <c r="A26" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="19"/>
+      <c r="T26" s="19"/>
+      <c r="U26" s="19"/>
+      <c r="V26" s="19"/>
+      <c r="W26" s="19"/>
+      <c r="X26" s="19"/>
+      <c r="Y26" s="19"/>
+      <c r="Z26" s="19"/>
     </row>
     <row r="27" ht="13.5" customHeight="1">
-      <c r="A27" s="8"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
+      <c r="A27" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="19"/>
+      <c r="U27" s="19"/>
+      <c r="V27" s="19"/>
+      <c r="W27" s="19"/>
+      <c r="X27" s="19"/>
+      <c r="Y27" s="19"/>
+      <c r="Z27" s="19"/>
     </row>
     <row r="28" ht="13.5" customHeight="1">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
+      <c r="A28" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="17"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="17"/>
+      <c r="Q28" s="17"/>
+      <c r="R28" s="17"/>
+      <c r="S28" s="17"/>
+      <c r="T28" s="17"/>
+      <c r="U28" s="17"/>
+      <c r="V28" s="17"/>
+      <c r="W28" s="17"/>
+      <c r="X28" s="17"/>
+      <c r="Y28" s="17"/>
+      <c r="Z28" s="17"/>
     </row>
     <row r="29" ht="13.5" customHeight="1">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="7"/>
-      <c r="O29" s="7"/>
+      <c r="A29" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17"/>
+      <c r="Q29" s="17"/>
+      <c r="R29" s="17"/>
+      <c r="S29" s="17"/>
+      <c r="T29" s="17"/>
+      <c r="U29" s="17"/>
+      <c r="V29" s="17"/>
+      <c r="W29" s="17"/>
+      <c r="X29" s="17"/>
+      <c r="Y29" s="17"/>
+      <c r="Z29" s="17"/>
     </row>
     <row r="30" ht="13.5" customHeight="1">
-      <c r="A30" s="12"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="7"/>
+      <c r="A30" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="17"/>
+      <c r="O30" s="17"/>
+      <c r="P30" s="17"/>
+      <c r="Q30" s="17"/>
+      <c r="R30" s="17"/>
+      <c r="S30" s="17"/>
+      <c r="T30" s="17"/>
+      <c r="U30" s="17"/>
+      <c r="V30" s="17"/>
+      <c r="W30" s="17"/>
+      <c r="X30" s="17"/>
+      <c r="Y30" s="17"/>
+      <c r="Z30" s="17"/>
     </row>
     <row r="31" ht="13.5" customHeight="1">
-      <c r="A31" s="3"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="7"/>
+      <c r="A31" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="17"/>
+      <c r="P31" s="17"/>
+      <c r="Q31" s="17"/>
+      <c r="R31" s="17"/>
+      <c r="S31" s="17"/>
+      <c r="T31" s="17"/>
+      <c r="U31" s="17"/>
+      <c r="V31" s="17"/>
+      <c r="W31" s="17"/>
+      <c r="X31" s="17"/>
+      <c r="Y31" s="17"/>
+      <c r="Z31" s="17"/>
     </row>
     <row r="32" ht="13.5" customHeight="1">
-      <c r="A32" s="3"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
+      <c r="A32" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
+      <c r="O32" s="17"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="17"/>
+      <c r="S32" s="17"/>
+      <c r="T32" s="17"/>
+      <c r="U32" s="17"/>
+      <c r="V32" s="17"/>
+      <c r="W32" s="17"/>
+      <c r="X32" s="17"/>
+      <c r="Y32" s="17"/>
+      <c r="Z32" s="17"/>
     </row>
     <row r="33" ht="13.5" customHeight="1">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="5"/>
-      <c r="N33" s="7"/>
-      <c r="O33" s="7"/>
+      <c r="A33" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="17"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="17"/>
+      <c r="Q33" s="17"/>
+      <c r="R33" s="17"/>
+      <c r="S33" s="17"/>
+      <c r="T33" s="17"/>
+      <c r="U33" s="17"/>
+      <c r="V33" s="17"/>
+      <c r="W33" s="17"/>
+      <c r="X33" s="17"/>
+      <c r="Y33" s="17"/>
+      <c r="Z33" s="17"/>
     </row>
     <row r="34" ht="13.5" customHeight="1">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
-      <c r="M34" s="5"/>
-      <c r="N34" s="7"/>
-      <c r="O34" s="7"/>
+      <c r="A34" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="17"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="17"/>
+      <c r="O34" s="17"/>
+      <c r="P34" s="17"/>
+      <c r="Q34" s="17"/>
+      <c r="R34" s="17"/>
+      <c r="S34" s="17"/>
+      <c r="T34" s="17"/>
+      <c r="U34" s="17"/>
+      <c r="V34" s="17"/>
+      <c r="W34" s="17"/>
+      <c r="X34" s="17"/>
+      <c r="Y34" s="17"/>
+      <c r="Z34" s="17"/>
     </row>
     <row r="35" ht="13.5" customHeight="1">
-      <c r="A35" s="3"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
-      <c r="M35" s="5"/>
-      <c r="N35" s="6"/>
-      <c r="O35" s="6"/>
+      <c r="A35" s="17"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="17"/>
+      <c r="N35" s="17"/>
+      <c r="O35" s="17"/>
+      <c r="P35" s="17"/>
+      <c r="Q35" s="17"/>
+      <c r="R35" s="17"/>
+      <c r="S35" s="17"/>
+      <c r="T35" s="17"/>
+      <c r="U35" s="17"/>
+      <c r="V35" s="17"/>
+      <c r="W35" s="17"/>
+      <c r="X35" s="17"/>
+      <c r="Y35" s="17"/>
+      <c r="Z35" s="17"/>
     </row>
     <row r="36" ht="13.5" customHeight="1">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="5"/>
-      <c r="N36" s="7"/>
-      <c r="O36" s="7"/>
+      <c r="A36" s="17"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="17"/>
+      <c r="N36" s="17"/>
+      <c r="O36" s="17"/>
+      <c r="P36" s="17"/>
+      <c r="Q36" s="17"/>
+      <c r="R36" s="17"/>
+      <c r="S36" s="17"/>
+      <c r="T36" s="17"/>
+      <c r="U36" s="17"/>
+      <c r="V36" s="17"/>
+      <c r="W36" s="17"/>
+      <c r="X36" s="17"/>
+      <c r="Y36" s="17"/>
+      <c r="Z36" s="17"/>
     </row>
     <row r="37" ht="13.5" customHeight="1">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="5"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="5"/>
-      <c r="N37" s="7"/>
-      <c r="O37" s="7"/>
-    </row>
-    <row r="38" ht="13.5" customHeight="1"/>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1"/>
+      <c r="A37" s="17"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="17"/>
+      <c r="K37" s="17"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="17"/>
+      <c r="N37" s="17"/>
+      <c r="O37" s="17"/>
+      <c r="P37" s="17"/>
+      <c r="Q37" s="17"/>
+      <c r="R37" s="17"/>
+      <c r="S37" s="17"/>
+      <c r="T37" s="17"/>
+      <c r="U37" s="17"/>
+      <c r="V37" s="17"/>
+      <c r="W37" s="17"/>
+      <c r="X37" s="17"/>
+      <c r="Y37" s="17"/>
+      <c r="Z37" s="17"/>
+    </row>
+    <row r="38" ht="13.5" customHeight="1">
+      <c r="A38" s="17"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="17"/>
+      <c r="K38" s="17"/>
+      <c r="L38" s="17"/>
+      <c r="M38" s="17"/>
+      <c r="N38" s="17"/>
+      <c r="O38" s="17"/>
+      <c r="P38" s="17"/>
+      <c r="Q38" s="17"/>
+      <c r="R38" s="17"/>
+      <c r="S38" s="17"/>
+      <c r="T38" s="17"/>
+      <c r="U38" s="17"/>
+      <c r="V38" s="17"/>
+      <c r="W38" s="17"/>
+      <c r="X38" s="17"/>
+      <c r="Y38" s="17"/>
+      <c r="Z38" s="17"/>
+    </row>
+    <row r="39" ht="13.5" customHeight="1">
+      <c r="A39" s="17"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="17"/>
+      <c r="K39" s="17"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="17"/>
+      <c r="O39" s="17"/>
+      <c r="P39" s="17"/>
+      <c r="Q39" s="17"/>
+      <c r="R39" s="17"/>
+      <c r="S39" s="17"/>
+      <c r="T39" s="17"/>
+      <c r="U39" s="17"/>
+      <c r="V39" s="17"/>
+      <c r="W39" s="17"/>
+      <c r="X39" s="17"/>
+      <c r="Y39" s="17"/>
+      <c r="Z39" s="17"/>
+    </row>
+    <row r="40" ht="13.5" customHeight="1">
+      <c r="A40" s="17"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
+      <c r="J40" s="17"/>
+      <c r="K40" s="17"/>
+      <c r="L40" s="17"/>
+      <c r="M40" s="17"/>
+      <c r="N40" s="17"/>
+      <c r="O40" s="17"/>
+      <c r="P40" s="17"/>
+      <c r="Q40" s="17"/>
+      <c r="R40" s="17"/>
+      <c r="S40" s="17"/>
+      <c r="T40" s="17"/>
+      <c r="U40" s="17"/>
+      <c r="V40" s="17"/>
+      <c r="W40" s="17"/>
+      <c r="X40" s="17"/>
+      <c r="Y40" s="17"/>
+      <c r="Z40" s="17"/>
+    </row>
+    <row r="41" ht="13.5" customHeight="1">
+      <c r="A41" s="17"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="17"/>
+      <c r="K41" s="17"/>
+      <c r="L41" s="17"/>
+      <c r="M41" s="17"/>
+      <c r="N41" s="17"/>
+      <c r="O41" s="17"/>
+      <c r="P41" s="17"/>
+      <c r="Q41" s="17"/>
+      <c r="R41" s="17"/>
+      <c r="S41" s="17"/>
+      <c r="T41" s="17"/>
+      <c r="U41" s="17"/>
+      <c r="V41" s="17"/>
+      <c r="W41" s="17"/>
+      <c r="X41" s="17"/>
+      <c r="Y41" s="17"/>
+      <c r="Z41" s="17"/>
+    </row>
+    <row r="42" ht="13.5" customHeight="1">
+      <c r="A42" s="17"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="17"/>
+      <c r="K42" s="17"/>
+      <c r="L42" s="17"/>
+      <c r="M42" s="17"/>
+      <c r="N42" s="17"/>
+      <c r="O42" s="17"/>
+      <c r="P42" s="17"/>
+      <c r="Q42" s="17"/>
+      <c r="R42" s="17"/>
+      <c r="S42" s="17"/>
+      <c r="T42" s="17"/>
+      <c r="U42" s="17"/>
+      <c r="V42" s="17"/>
+      <c r="W42" s="17"/>
+      <c r="X42" s="17"/>
+      <c r="Y42" s="17"/>
+      <c r="Z42" s="17"/>
+    </row>
+    <row r="43" ht="13.5" customHeight="1">
+      <c r="A43" s="17"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="17"/>
+      <c r="K43" s="17"/>
+      <c r="L43" s="17"/>
+      <c r="M43" s="17"/>
+      <c r="N43" s="17"/>
+      <c r="O43" s="17"/>
+      <c r="P43" s="17"/>
+      <c r="Q43" s="17"/>
+      <c r="R43" s="17"/>
+      <c r="S43" s="17"/>
+      <c r="T43" s="17"/>
+      <c r="U43" s="17"/>
+      <c r="V43" s="17"/>
+      <c r="W43" s="17"/>
+      <c r="X43" s="17"/>
+      <c r="Y43" s="17"/>
+      <c r="Z43" s="17"/>
+    </row>
+    <row r="44" ht="13.5" customHeight="1">
+      <c r="A44" s="17"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17"/>
+      <c r="K44" s="17"/>
+      <c r="L44" s="17"/>
+      <c r="M44" s="17"/>
+      <c r="N44" s="17"/>
+      <c r="O44" s="17"/>
+      <c r="P44" s="17"/>
+      <c r="Q44" s="17"/>
+      <c r="R44" s="17"/>
+      <c r="S44" s="17"/>
+      <c r="T44" s="17"/>
+      <c r="U44" s="17"/>
+      <c r="V44" s="17"/>
+      <c r="W44" s="17"/>
+      <c r="X44" s="17"/>
+      <c r="Y44" s="17"/>
+      <c r="Z44" s="17"/>
+    </row>
+    <row r="45" ht="13.5" customHeight="1">
+      <c r="A45" s="17"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="17"/>
+      <c r="J45" s="17"/>
+      <c r="K45" s="17"/>
+      <c r="L45" s="17"/>
+      <c r="M45" s="17"/>
+      <c r="N45" s="17"/>
+      <c r="O45" s="17"/>
+      <c r="P45" s="17"/>
+      <c r="Q45" s="17"/>
+      <c r="R45" s="17"/>
+      <c r="S45" s="17"/>
+      <c r="T45" s="17"/>
+      <c r="U45" s="17"/>
+      <c r="V45" s="17"/>
+      <c r="W45" s="17"/>
+      <c r="X45" s="17"/>
+      <c r="Y45" s="17"/>
+      <c r="Z45" s="17"/>
+    </row>
+    <row r="46" ht="13.5" customHeight="1">
+      <c r="A46" s="17"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="17"/>
+      <c r="K46" s="17"/>
+      <c r="L46" s="17"/>
+      <c r="M46" s="17"/>
+      <c r="N46" s="17"/>
+      <c r="O46" s="17"/>
+      <c r="P46" s="17"/>
+      <c r="Q46" s="17"/>
+      <c r="R46" s="17"/>
+      <c r="S46" s="17"/>
+      <c r="T46" s="17"/>
+      <c r="U46" s="17"/>
+      <c r="V46" s="17"/>
+      <c r="W46" s="17"/>
+      <c r="X46" s="17"/>
+      <c r="Y46" s="17"/>
+      <c r="Z46" s="17"/>
+    </row>
+    <row r="47" ht="13.5" customHeight="1">
+      <c r="A47" s="17"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="17"/>
+      <c r="K47" s="17"/>
+      <c r="L47" s="17"/>
+      <c r="M47" s="17"/>
+      <c r="N47" s="17"/>
+      <c r="O47" s="17"/>
+      <c r="P47" s="17"/>
+      <c r="Q47" s="17"/>
+      <c r="R47" s="17"/>
+      <c r="S47" s="17"/>
+      <c r="T47" s="17"/>
+      <c r="U47" s="17"/>
+      <c r="V47" s="17"/>
+      <c r="W47" s="17"/>
+      <c r="X47" s="17"/>
+      <c r="Y47" s="17"/>
+      <c r="Z47" s="17"/>
+    </row>
+    <row r="48" ht="13.5" customHeight="1">
+      <c r="A48" s="17"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="17"/>
+      <c r="J48" s="17"/>
+      <c r="K48" s="17"/>
+      <c r="L48" s="17"/>
+      <c r="M48" s="17"/>
+      <c r="N48" s="17"/>
+      <c r="O48" s="17"/>
+      <c r="P48" s="17"/>
+      <c r="Q48" s="17"/>
+      <c r="R48" s="17"/>
+      <c r="S48" s="17"/>
+      <c r="T48" s="17"/>
+      <c r="U48" s="17"/>
+      <c r="V48" s="17"/>
+      <c r="W48" s="17"/>
+      <c r="X48" s="17"/>
+      <c r="Y48" s="17"/>
+      <c r="Z48" s="17"/>
+    </row>
+    <row r="49" ht="13.5" customHeight="1">
+      <c r="A49" s="17"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
+      <c r="I49" s="17"/>
+      <c r="J49" s="17"/>
+      <c r="K49" s="17"/>
+      <c r="L49" s="17"/>
+      <c r="M49" s="17"/>
+      <c r="N49" s="17"/>
+      <c r="O49" s="17"/>
+      <c r="P49" s="17"/>
+      <c r="Q49" s="17"/>
+      <c r="R49" s="17"/>
+      <c r="S49" s="17"/>
+      <c r="T49" s="17"/>
+      <c r="U49" s="17"/>
+      <c r="V49" s="17"/>
+      <c r="W49" s="17"/>
+      <c r="X49" s="17"/>
+      <c r="Y49" s="17"/>
+      <c r="Z49" s="17"/>
+    </row>
+    <row r="50" ht="13.5" customHeight="1">
+      <c r="A50" s="17"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
+      <c r="J50" s="17"/>
+      <c r="K50" s="17"/>
+      <c r="L50" s="17"/>
+      <c r="M50" s="17"/>
+      <c r="N50" s="17"/>
+      <c r="O50" s="17"/>
+      <c r="P50" s="17"/>
+      <c r="Q50" s="17"/>
+      <c r="R50" s="17"/>
+      <c r="S50" s="17"/>
+      <c r="T50" s="17"/>
+      <c r="U50" s="17"/>
+      <c r="V50" s="17"/>
+      <c r="W50" s="17"/>
+      <c r="X50" s="17"/>
+      <c r="Y50" s="17"/>
+      <c r="Z50" s="17"/>
+    </row>
+    <row r="51" ht="13.5" customHeight="1">
+      <c r="A51" s="17"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="17"/>
+      <c r="I51" s="17"/>
+      <c r="J51" s="17"/>
+      <c r="K51" s="17"/>
+      <c r="L51" s="17"/>
+      <c r="M51" s="17"/>
+      <c r="N51" s="17"/>
+      <c r="O51" s="17"/>
+      <c r="P51" s="17"/>
+      <c r="Q51" s="17"/>
+      <c r="R51" s="17"/>
+      <c r="S51" s="17"/>
+      <c r="T51" s="17"/>
+      <c r="U51" s="17"/>
+      <c r="V51" s="17"/>
+      <c r="W51" s="17"/>
+      <c r="X51" s="17"/>
+      <c r="Y51" s="17"/>
+      <c r="Z51" s="17"/>
+    </row>
     <row r="52" ht="15.75" customHeight="1"/>
     <row r="53" ht="15.75" customHeight="1"/>
     <row r="54" ht="15.75" customHeight="1"/>
@@ -1973,14 +2722,13 @@
     <row r="988" ht="15.75" customHeight="1"/>
     <row r="989" ht="15.75" customHeight="1"/>
     <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="1">
     <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A16:C16"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -2005,79 +2753,79 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added new test cases with It's functions for Make A Copy.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/makeACopy_newUI/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/makeACopy_newUI/TestData.xlsx
@@ -12,12 +12,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="81">
+  <si>
+    <t>Supported Browser Types</t>
+  </si>
   <si>
     <t>Variable</t>
   </si>
   <si>
-    <t>Supported Browser Types</t>
+    <t>MozillaFirefox</t>
+  </si>
+  <si>
+    <t>GoogleChrome</t>
+  </si>
+  <si>
+    <t>MicrosoftInternetExplorer</t>
+  </si>
+  <si>
+    <t>MicrosoftEdge</t>
   </si>
   <si>
     <t>Data1</t>
@@ -35,18 +47,6 @@
     <t>URL_login_login</t>
   </si>
   <si>
-    <t>MozillaFirefox</t>
-  </si>
-  <si>
-    <t>GoogleChrome</t>
-  </si>
-  <si>
-    <t>MicrosoftInternetExplorer</t>
-  </si>
-  <si>
-    <t>MicrosoftEdge</t>
-  </si>
-  <si>
     <t>#/login</t>
   </si>
   <si>
@@ -222,13 +222,46 @@
   </si>
   <si>
     <t>New Folder Created by admin and shared 'Share' to analyzer</t>
+  </si>
+  <si>
+    <t>Automation_Folder_Inside_AutomationFolder</t>
+  </si>
+  <si>
+    <t>New Folder created inside folder "Automation_Folder_ToCopyDashboardToIt"</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_CopiedAndFoundInSearch</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_DuplicateError Copy</t>
+  </si>
+  <si>
+    <t>New dashboard created inside folder "Automation_Folder_ToCopyDashboardToIt"</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_DuplicateError</t>
+  </si>
+  <si>
+    <t>Automation_Folder_Copy1</t>
+  </si>
+  <si>
+    <t>Automation_Folder_Copy2</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_Copy1</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_Copy2</t>
+  </si>
+  <si>
+    <t>New Dashboard exist in "Automation_Folder_Copy2"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -254,6 +287,11 @@
     <font>
       <sz val="11.0"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Docs-Calibri"/>
     </font>
   </fonts>
   <fills count="5">
@@ -338,15 +376,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -401,6 +439,9 @@
     <xf borderId="0" fillId="4" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -435,35 +476,35 @@
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
     </row>
     <row r="2" ht="13.5" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>11</v>
@@ -1308,9 +1349,15 @@
       <c r="Z34" s="17"/>
     </row>
     <row r="35" ht="13.5" customHeight="1">
-      <c r="A35" s="17"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
+      <c r="A35" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>71</v>
+      </c>
       <c r="D35" s="17"/>
       <c r="E35" s="17"/>
       <c r="F35" s="17"/>
@@ -1336,9 +1383,15 @@
       <c r="Z35" s="17"/>
     </row>
     <row r="36" ht="13.5" customHeight="1">
-      <c r="A36" s="17"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
+      <c r="A36" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>38</v>
+      </c>
       <c r="D36" s="17"/>
       <c r="E36" s="17"/>
       <c r="F36" s="17"/>
@@ -1364,9 +1417,15 @@
       <c r="Z36" s="17"/>
     </row>
     <row r="37" ht="13.5" customHeight="1">
-      <c r="A37" s="17"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="17"/>
+      <c r="A37" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="D37" s="17"/>
       <c r="E37" s="17"/>
       <c r="F37" s="17"/>
@@ -1392,9 +1451,15 @@
       <c r="Z37" s="17"/>
     </row>
     <row r="38" ht="13.5" customHeight="1">
-      <c r="A38" s="17"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
+      <c r="A38" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>38</v>
+      </c>
       <c r="D38" s="17"/>
       <c r="E38" s="17"/>
       <c r="F38" s="17"/>
@@ -1420,9 +1485,15 @@
       <c r="Z38" s="17"/>
     </row>
     <row r="39" ht="13.5" customHeight="1">
-      <c r="A39" s="17"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
+      <c r="A39" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>40</v>
+      </c>
       <c r="D39" s="17"/>
       <c r="E39" s="17"/>
       <c r="F39" s="17"/>
@@ -1448,9 +1519,15 @@
       <c r="Z39" s="17"/>
     </row>
     <row r="40" ht="13.5" customHeight="1">
-      <c r="A40" s="17"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
+      <c r="A40" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>40</v>
+      </c>
       <c r="D40" s="17"/>
       <c r="E40" s="17"/>
       <c r="F40" s="17"/>
@@ -1476,9 +1553,15 @@
       <c r="Z40" s="17"/>
     </row>
     <row r="41" ht="13.5" customHeight="1">
-      <c r="A41" s="17"/>
-      <c r="B41" s="17"/>
-      <c r="C41" s="17"/>
+      <c r="A41" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>38</v>
+      </c>
       <c r="D41" s="17"/>
       <c r="E41" s="17"/>
       <c r="F41" s="17"/>
@@ -1504,9 +1587,15 @@
       <c r="Z41" s="17"/>
     </row>
     <row r="42" ht="13.5" customHeight="1">
-      <c r="A42" s="17"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="17"/>
+      <c r="A42" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>80</v>
+      </c>
       <c r="D42" s="17"/>
       <c r="E42" s="17"/>
       <c r="F42" s="17"/>
@@ -2753,79 +2842,79 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Finalizing creation of TCs in class NewUI_MakACopy.java Updating Functions in class NewUI_Content.java Updating TestData.xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/makeACopy_newUI/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/makeACopy_newUI/TestData.xlsx
@@ -12,11 +12,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="85">
+  <si>
+    <t>Supported Browser Types</t>
+  </si>
   <si>
     <t>Variable</t>
   </si>
   <si>
+    <t>MozillaFirefox</t>
+  </si>
+  <si>
+    <t>GoogleChrome</t>
+  </si>
+  <si>
+    <t>MicrosoftInternetExplorer</t>
+  </si>
+  <si>
+    <t>MicrosoftEdge</t>
+  </si>
+  <si>
     <t>Data1</t>
   </si>
   <si>
@@ -92,7 +107,7 @@
     <t>Tenant</t>
   </si>
   <si>
-    <t>demo</t>
+    <t>content_test</t>
   </si>
   <si>
     <t>Username</t>
@@ -104,7 +119,7 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Automation_Analyzer1</t>
+    <t>Automation_Analyzer11</t>
   </si>
   <si>
     <t>Comments</t>
@@ -128,33 +143,18 @@
     <t>Automation_Dashboard_Copy</t>
   </si>
   <si>
-    <t>Supported Browser Types</t>
-  </si>
-  <si>
     <t>Automation_Dashboard_CancelCopy</t>
   </si>
   <si>
-    <t>MozillaFirefox</t>
-  </si>
-  <si>
     <t>Automation_Dashboard_CopyDashboard_LongDashboardName</t>
   </si>
   <si>
-    <t>GoogleChrome</t>
-  </si>
-  <si>
     <t>LongDashboardName</t>
   </si>
   <si>
-    <t>MicrosoftInternetExplorer</t>
-  </si>
-  <si>
     <t>Automation_Dashboard_CopyDashboard_LongDashboardNameAutomation_Dashboard_CopyDashboard_LongDashboardNameAutomation_Dashboard_CopyDashboard_LongDashboardNameAutomation_Dashboard_CopyDashboard_LongDashboardName</t>
   </si>
   <si>
-    <t>MicrosoftEdge</t>
-  </si>
-  <si>
     <t>New Long Dashboard Name</t>
   </si>
   <si>
@@ -264,13 +264,16 @@
   </si>
   <si>
     <t>Automation_Folder_SelectedByDefaultInCopyScreen</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_Copy_NamingConvention</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -296,11 +299,6 @@
     <font>
       <sz val="11.0"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
-      <name val="Docs-Calibri"/>
     </font>
   </fonts>
   <fills count="5">
@@ -385,9 +383,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -421,9 +422,6 @@
     <xf borderId="5" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
@@ -446,9 +444,6 @@
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -485,503 +480,503 @@
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
     </row>
     <row r="2" ht="13.5" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
     </row>
     <row r="3" ht="13.5" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
     </row>
     <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
     </row>
     <row r="5" ht="13.5" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
     </row>
     <row r="6" ht="13.5" customHeight="1">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
     </row>
     <row r="7" ht="13.5" customHeight="1">
-      <c r="A7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
     </row>
     <row r="8" ht="13.5" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
+      <c r="A8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
     </row>
     <row r="9" ht="13.5" customHeight="1">
-      <c r="A9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
+      <c r="A9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
     </row>
     <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
+      <c r="A10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
     </row>
     <row r="11" ht="13.5" customHeight="1">
-      <c r="A11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
+      <c r="A11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
     </row>
     <row r="12" ht="13.5" customHeight="1">
-      <c r="A12" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
+      <c r="A12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
     </row>
     <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
+      <c r="A13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
     </row>
     <row r="14" ht="13.5" customHeight="1">
-      <c r="A14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
+      <c r="A14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
     </row>
     <row r="15" ht="13.5" customHeight="1">
-      <c r="A15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
+      <c r="A15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
     </row>
     <row r="16" ht="13.5" customHeight="1">
-      <c r="A16" s="7"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
     </row>
     <row r="17" ht="13.5" customHeight="1">
-      <c r="A17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
+      <c r="A17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
     </row>
     <row r="18" ht="13.5" customHeight="1">
-      <c r="A18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
+      <c r="A18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
     </row>
     <row r="19" ht="13.5" customHeight="1">
-      <c r="A19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
+      <c r="A19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
     </row>
     <row r="20" ht="13.5" customHeight="1">
-      <c r="A20" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
+      <c r="A20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
     </row>
     <row r="21" ht="13.5" customHeight="1">
-      <c r="A21" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
+      <c r="A21" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
     </row>
     <row r="22" ht="13.5" customHeight="1">
-      <c r="A22" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
+      <c r="A22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
     </row>
     <row r="23" ht="13.5" customHeight="1">
-      <c r="A23" s="2" t="s">
-        <v>43</v>
+      <c r="A23" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="A24" s="15" t="s">
@@ -991,7 +986,7 @@
         <v>48</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
@@ -1059,7 +1054,7 @@
         <v>52</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
@@ -1127,7 +1122,7 @@
         <v>56</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
@@ -1195,7 +1190,7 @@
         <v>60</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D30" s="17"/>
       <c r="E30" s="17"/>
@@ -1399,7 +1394,7 @@
         <v>72</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D36" s="17"/>
       <c r="E36" s="17"/>
@@ -1467,7 +1462,7 @@
         <v>75</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D38" s="17"/>
       <c r="E38" s="17"/>
@@ -1501,7 +1496,7 @@
         <v>76</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D39" s="17"/>
       <c r="E39" s="17"/>
@@ -1535,7 +1530,7 @@
         <v>77</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D40" s="17"/>
       <c r="E40" s="17"/>
@@ -1569,7 +1564,7 @@
         <v>78</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D41" s="17"/>
       <c r="E41" s="17"/>
@@ -1599,7 +1594,7 @@
       <c r="A42" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="B42" s="22" t="s">
+      <c r="B42" s="21" t="s">
         <v>79</v>
       </c>
       <c r="C42" s="16" t="s">
@@ -1671,7 +1666,7 @@
         <v>83</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D44" s="17"/>
       <c r="E44" s="17"/>
@@ -1698,9 +1693,15 @@
       <c r="Z44" s="17"/>
     </row>
     <row r="45" ht="13.5" customHeight="1">
-      <c r="A45" s="17"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="17"/>
+      <c r="A45" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>38</v>
+      </c>
       <c r="D45" s="17"/>
       <c r="E45" s="17"/>
       <c r="F45" s="17"/>
@@ -2863,79 +2864,79 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
     </row>
     <row r="2">
-      <c r="A2" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
     <row r="3">
-      <c r="A3" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
     </row>
     <row r="4">
-      <c r="A4" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>